<commit_message>
Add utils.go, auto upper initial character for all fields
</commit_message>
<xml_diff>
--- a/excels/simple_types.xlsx
+++ b/excels/simple_types.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="110">
   <si>
     <t>KEY</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>//</t>
+  </si>
+  <si>
+    <t>dictTest1</t>
   </si>
 </sst>
 </file>
@@ -819,7 +822,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,7 +976,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="13" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>13</v>

</xml_diff>